<commit_message>
change the path of the excel files
</commit_message>
<xml_diff>
--- a/Resources/Checkoutform.xlsx
+++ b/Resources/Checkoutform.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Desktop\SauceDemo-Project\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5232D314-83AB-4232-9EE9-06A65139C62F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B17F4B65-C416-4331-80AF-986C36F7FD3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2304" yWindow="2304" windowWidth="6360" windowHeight="8880" xr2:uid="{C5E426E0-C1E5-4AB8-8D20-FA80383C92D1}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{C5E426E0-C1E5-4AB8-8D20-FA80383C92D1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="5">
   <si>
     <t>${firstname}</t>
   </si>
@@ -400,10 +400,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB62007C-627E-48AF-906D-8CFC56FD62F2}">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -445,19 +445,27 @@
         <v>36524</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B7" t="s">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B6" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>3</v>
-      </c>
       <c r="B8" t="s">
         <v>4</v>
       </c>
       <c r="C8">
+        <v>63258</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>3</v>
+      </c>
+      <c r="B9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9">
         <v>632589</v>
       </c>
     </row>

</xml_diff>